<commit_message>
start move to MaxEnt2018.py
commit for reference - no changes yet in central calculation
</commit_message>
<xml_diff>
--- a/Tester.xlsx
+++ b/Tester.xlsx
@@ -468,46 +468,46 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>61.88464666346164</v>
+        <v>9.620941820144424</v>
       </c>
       <c r="C2">
-        <v>27.48249458796555</v>
+        <v>111.7799371981589</v>
       </c>
       <c r="D2">
-        <v>-5.246862582180719e-05</v>
+        <v>-45.88718780204495</v>
       </c>
       <c r="E2">
-        <v>-269.885290562501</v>
+        <v>0.5316223109327038</v>
       </c>
       <c r="F2">
-        <v>-0.3445088882654737</v>
+        <v>0.1394445509794191</v>
       </c>
       <c r="G2">
-        <v>0.2246000830688568</v>
+        <v>-0.5048984562177226</v>
       </c>
       <c r="H2">
-        <v>1.434952644141952</v>
+        <v>-0.2887852418321486</v>
       </c>
       <c r="I2">
-        <v>0.02509128431958496</v>
+        <v>0.5882320493937718</v>
       </c>
       <c r="J2">
-        <v>4.355252456382743</v>
+        <v>4.35380751296719</v>
       </c>
       <c r="K2">
-        <v>69</v>
+        <v>810</v>
       </c>
       <c r="L2">
-        <v>219.5782601303623</v>
+        <v>-18.48992474722918</v>
       </c>
       <c r="M2">
         <v>0</v>
       </c>
       <c r="N2">
-        <v>4.355252456382715</v>
+        <v>4.355733271500807</v>
       </c>
       <c r="O2">
-        <v>5.021919123049382</v>
+        <v>5.022399938167474</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -515,46 +515,46 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>-140.5554998812986</v>
+        <v>13.70805124018053</v>
       </c>
       <c r="C3">
-        <v>-0.08662494730567394</v>
+        <v>73.57141012288875</v>
       </c>
       <c r="D3">
-        <v>38.88782270075285</v>
+        <v>1.136323524991484</v>
       </c>
       <c r="E3">
-        <v>115.519938395257</v>
+        <v>-0.004722624389567093</v>
       </c>
       <c r="F3">
-        <v>0.30900531174423</v>
+        <v>-0.09075079051307866</v>
       </c>
       <c r="G3">
-        <v>0.9419202902581456</v>
+        <v>-0.8046956967412628</v>
       </c>
       <c r="H3">
-        <v>-0.8435650017629155</v>
+        <v>0.560927550153024</v>
       </c>
       <c r="I3">
-        <v>0.3431592867194002</v>
+        <v>1.119291812005977</v>
       </c>
       <c r="J3">
-        <v>4.35525605717924</v>
+        <v>4.35382222130746</v>
       </c>
       <c r="K3">
-        <v>13</v>
+        <v>947</v>
       </c>
       <c r="L3">
-        <v>34.65021179594592</v>
+        <v>-18.49010939143442</v>
       </c>
       <c r="M3">
         <v>0</v>
       </c>
       <c r="N3">
-        <v>4.355256057179332</v>
+        <v>4.355790627299218</v>
       </c>
       <c r="O3">
-        <v>5.021922723845999</v>
+        <v>5.022457293965885</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -562,46 +562,46 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>4.984168381423277</v>
+        <v>4.881855501439038e-05</v>
       </c>
       <c r="C4">
-        <v>0.7422792626513783</v>
+        <v>-15.59355872078886</v>
       </c>
       <c r="D4">
-        <v>55.48355443501079</v>
+        <v>91.89455332265962</v>
       </c>
       <c r="E4">
-        <v>-0.002913335297259918</v>
+        <v>5.060803157519546</v>
       </c>
       <c r="F4">
-        <v>-0.08816067962178398</v>
+        <v>1.908531899953754</v>
       </c>
       <c r="G4">
-        <v>0.6500292937543453</v>
+        <v>-0.980498000492672</v>
       </c>
       <c r="H4">
-        <v>-0.5840020451438213</v>
+        <v>-0.6838360209790908</v>
       </c>
       <c r="I4">
-        <v>1.330091947399709</v>
+        <v>0.3214507537716988</v>
       </c>
       <c r="J4">
-        <v>4.355269354901294</v>
+        <v>4.35373034338852</v>
       </c>
       <c r="K4">
-        <v>15</v>
+        <v>274</v>
       </c>
       <c r="L4">
-        <v>-13.99721201823534</v>
+        <v>-19.77182838957472</v>
       </c>
       <c r="M4">
         <v>0</v>
       </c>
       <c r="N4">
-        <v>4.355269353098812</v>
+        <v>4.355831438025106</v>
       </c>
       <c r="O4">
-        <v>5.021936019765479</v>
+        <v>5.022498104691773</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -609,46 +609,46 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>1.731089741819137</v>
+        <v>-18.79572377302581</v>
       </c>
       <c r="C5">
-        <v>-20.88145507133931</v>
+        <v>108.0143304883464</v>
       </c>
       <c r="D5">
-        <v>56.74358984291425</v>
+        <v>82.58560653467021</v>
       </c>
       <c r="E5">
-        <v>0.9331601849973978</v>
+        <v>0.0206616990655788</v>
       </c>
       <c r="F5">
-        <v>0.435953996012056</v>
+        <v>-0.3944535604316779</v>
       </c>
       <c r="G5">
-        <v>0.08460181383262277</v>
+        <v>-0.5515785120814303</v>
       </c>
       <c r="H5">
-        <v>-0.6539967747003432</v>
+        <v>0.05761981773850167</v>
       </c>
       <c r="I5">
-        <v>0.4835575699329313</v>
+        <v>1.035222800523765</v>
       </c>
       <c r="J5">
-        <v>4.355323685649539</v>
+        <v>4.353718927559044</v>
       </c>
       <c r="K5">
-        <v>11</v>
+        <v>666</v>
       </c>
       <c r="L5">
-        <v>13.05983235539085</v>
+        <v>-109.0138359232274</v>
       </c>
       <c r="M5">
         <v>0</v>
       </c>
       <c r="N5">
-        <v>4.355323685649541</v>
+        <v>4.355874682681559</v>
       </c>
       <c r="O5">
-        <v>5.021990352316208</v>
+        <v>5.022541349348226</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -656,46 +656,46 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>22.59667622005085</v>
+        <v>71.94057355310238</v>
       </c>
       <c r="C6">
-        <v>70.57790757314554</v>
+        <v>32.22058039594563</v>
       </c>
       <c r="D6">
-        <v>-0.5340835471661796</v>
+        <v>0.0001373789959456304</v>
       </c>
       <c r="E6">
-        <v>1.52274429817475</v>
+        <v>146.6625828325254</v>
       </c>
       <c r="F6">
-        <v>-1.088673983314165</v>
+        <v>-1.166152362930291</v>
       </c>
       <c r="G6">
-        <v>-0.1536034893097724</v>
+        <v>0.1893305969037313</v>
       </c>
       <c r="H6">
-        <v>0.9275025091984599</v>
+        <v>1.685687279781414</v>
       </c>
       <c r="I6">
-        <v>0.7924208937731749</v>
+        <v>-0.1049567099281041</v>
       </c>
       <c r="J6">
-        <v>4.354465448367058</v>
+        <v>4.353816357952695</v>
       </c>
       <c r="K6">
-        <v>58</v>
+        <v>441</v>
       </c>
       <c r="L6">
-        <v>-48.62894688910129</v>
+        <v>-161.5994162031472</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
       <c r="N6">
-        <v>4.355331006002785</v>
+        <v>4.355906907589571</v>
       </c>
       <c r="O6">
-        <v>5.021997672669452</v>
+        <v>5.022573574256238</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -703,46 +703,46 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>111.5618426474662</v>
+        <v>15.01760889926723</v>
       </c>
       <c r="C7">
-        <v>0.770185678579651</v>
+        <v>83.35191320937608</v>
       </c>
       <c r="D7">
-        <v>-0.3009565899678053</v>
+        <v>0.0006261238700516225</v>
       </c>
       <c r="E7">
-        <v>-46.38533784481443</v>
+        <v>82.72617323457345</v>
       </c>
       <c r="F7">
-        <v>-0.7458380628260872</v>
+        <v>-0.6946099860784332</v>
       </c>
       <c r="G7">
-        <v>0.7490369095636624</v>
+        <v>-0.4954437038043416</v>
       </c>
       <c r="H7">
-        <v>0.8263341495074008</v>
+        <v>1.574032491211521</v>
       </c>
       <c r="I7">
-        <v>-0.7601301287639288</v>
+        <v>0.07315505356854901</v>
       </c>
       <c r="J7">
-        <v>4.35539535373389</v>
+        <v>4.353690067355402</v>
       </c>
       <c r="K7">
-        <v>23</v>
+        <v>186</v>
       </c>
       <c r="L7">
-        <v>-6.360846808962469</v>
+        <v>-119.3163241619844</v>
       </c>
       <c r="M7">
         <v>0</v>
       </c>
       <c r="N7">
-        <v>4.355395353737206</v>
+        <v>4.355930353028171</v>
       </c>
       <c r="O7">
-        <v>5.022062020403873</v>
+        <v>5.022597019694838</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -750,46 +750,46 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>-28.06871755351681</v>
+        <v>63.85248572969289</v>
       </c>
       <c r="C8">
-        <v>24.29399996467725</v>
+        <v>1.445582801208831</v>
       </c>
       <c r="D8">
-        <v>0.8970093144674914</v>
+        <v>19.90509115604056</v>
       </c>
       <c r="E8">
-        <v>75.43572545302592</v>
+        <v>15.64103335126555</v>
       </c>
       <c r="F8">
-        <v>-0.8990909219655483</v>
+        <v>-0.838818744605369</v>
       </c>
       <c r="G8">
-        <v>-0.361535937452766</v>
+        <v>0.5069442129442572</v>
       </c>
       <c r="H8">
-        <v>0.5842696008819024</v>
+        <v>-1.199429697840287</v>
       </c>
       <c r="I8">
-        <v>-0.9061372565873638</v>
+        <v>-0.1271970609481965</v>
       </c>
       <c r="J8">
-        <v>4.355398380954323</v>
+        <v>4.353794088132723</v>
       </c>
       <c r="K8">
-        <v>22</v>
+        <v>801</v>
       </c>
       <c r="L8">
-        <v>-11.97497597636353</v>
+        <v>-18.48975571815647</v>
       </c>
       <c r="M8">
         <v>0</v>
       </c>
       <c r="N8">
-        <v>4.355398374547054</v>
+        <v>4.355956415020117</v>
       </c>
       <c r="O8">
-        <v>5.022065041213721</v>
+        <v>5.022623081686784</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -797,46 +797,46 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>-68.6665328994668</v>
+        <v>-10.67969568839464</v>
       </c>
       <c r="C9">
-        <v>-9.731644767779251</v>
+        <v>0.069971217097127</v>
       </c>
       <c r="D9">
-        <v>12.51025989633819</v>
+        <v>7.161349042059957</v>
       </c>
       <c r="E9">
-        <v>122.0808768110439</v>
+        <v>93.20732053430905</v>
       </c>
       <c r="F9">
-        <v>-0.2012302099540637</v>
+        <v>-0.4610328246617112</v>
       </c>
       <c r="G9">
-        <v>0.4345620499696121</v>
+        <v>0.8571344113150654</v>
       </c>
       <c r="H9">
-        <v>0.4358671446101017</v>
+        <v>0.2130926335193486</v>
       </c>
       <c r="I9">
-        <v>-0.2965573622859135</v>
+        <v>-0.7067080165397148</v>
       </c>
       <c r="J9">
-        <v>4.354558646454517</v>
+        <v>4.353734053836256</v>
       </c>
       <c r="K9">
-        <v>90</v>
+        <v>219</v>
       </c>
       <c r="L9">
-        <v>-18.4944131410288</v>
+        <v>-18.48998246241425</v>
       </c>
       <c r="M9">
         <v>0</v>
       </c>
       <c r="N9">
-        <v>4.355421716731566</v>
+        <v>4.355977773038699</v>
       </c>
       <c r="O9">
-        <v>5.022088383398233</v>
+        <v>5.022644439705366</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -844,46 +844,46 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>-12.99565777078672</v>
+        <v>12.59202612535058</v>
       </c>
       <c r="C10">
-        <v>71.18372270212365</v>
+        <v>2.949494921891286</v>
       </c>
       <c r="D10">
-        <v>6.971129631873378</v>
+        <v>0.2559593421907637</v>
       </c>
       <c r="E10">
-        <v>0.448380184362597</v>
+        <v>82.92236675692584</v>
       </c>
       <c r="F10">
-        <v>-0.6053838460646812</v>
+        <v>-0.1587343389394977</v>
       </c>
       <c r="G10">
-        <v>-0.7141655668480422</v>
+        <v>0.298164239586872</v>
       </c>
       <c r="H10">
-        <v>-0.9354361681350911</v>
+        <v>0.6808302357053031</v>
       </c>
       <c r="I10">
-        <v>0.6786403660710691</v>
+        <v>-0.8756000411091078</v>
       </c>
       <c r="J10">
-        <v>4.355449791179572</v>
+        <v>4.353766400874147</v>
       </c>
       <c r="K10">
-        <v>28</v>
+        <v>197</v>
       </c>
       <c r="L10">
-        <v>-5.599154025823309</v>
+        <v>-18.50061651607908</v>
       </c>
       <c r="M10">
         <v>0</v>
       </c>
       <c r="N10">
-        <v>4.355449791183356</v>
+        <v>4.356025606750617</v>
       </c>
       <c r="O10">
-        <v>5.022116457850023</v>
+        <v>5.022692273417284</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -891,46 +891,46 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>40.42830180080568</v>
+        <v>76.16162303422527</v>
       </c>
       <c r="C11">
-        <v>239.6733307534205</v>
+        <v>120.8958378571488</v>
       </c>
       <c r="D11">
-        <v>-286.1489724380541</v>
+        <v>38.71805380907443</v>
       </c>
       <c r="E11">
-        <v>-0.1368467443258629</v>
+        <v>0.06937189547648326</v>
       </c>
       <c r="F11">
-        <v>-1.88126585315716</v>
+        <v>-0.8237584855118192</v>
       </c>
       <c r="G11">
-        <v>0.3319743836048055</v>
+        <v>0.0430167232194969</v>
       </c>
       <c r="H11">
-        <v>0.3031922693291742</v>
+        <v>-0.2269302406879004</v>
       </c>
       <c r="I11">
-        <v>0.9611289982445004</v>
+        <v>0.8737592316565159</v>
       </c>
       <c r="J11">
-        <v>4.355530942731917</v>
+        <v>4.353730130279445</v>
       </c>
       <c r="K11">
-        <v>45</v>
+        <v>994</v>
       </c>
       <c r="L11">
-        <v>68.57141473354073</v>
+        <v>-160.0330460197437</v>
       </c>
       <c r="M11">
         <v>0</v>
       </c>
       <c r="N11">
-        <v>4.35553094272953</v>
+        <v>4.356025841023182</v>
       </c>
       <c r="O11">
-        <v>5.022197609396197</v>
+        <v>5.022692507689849</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating for flexible input data and auto-syntax
WIP - testrun 22h15 MCS data Aakash on single purpose worker
</commit_message>
<xml_diff>
--- a/Tester.xlsx
+++ b/Tester.xlsx
@@ -468,46 +468,46 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>9.620941820144424</v>
+        <v>0.007921659358885036</v>
       </c>
       <c r="C2">
-        <v>111.7799371981589</v>
+        <v>104.7277239638582</v>
       </c>
       <c r="D2">
-        <v>-45.88718780204495</v>
+        <v>-76.12851921821058</v>
       </c>
       <c r="E2">
-        <v>0.5316223109327038</v>
+        <v>86.83826899324438</v>
       </c>
       <c r="F2">
-        <v>0.1394445509794191</v>
+        <v>1.087736738464413</v>
       </c>
       <c r="G2">
-        <v>-0.5048984562177226</v>
+        <v>0.137925699246686</v>
       </c>
       <c r="H2">
-        <v>-0.2887852418321486</v>
+        <v>0.1321353430312686</v>
       </c>
       <c r="I2">
-        <v>0.5882320493937718</v>
+        <v>-0.457978408653416</v>
       </c>
       <c r="J2">
-        <v>4.35380751296719</v>
+        <v>4.353809811669684</v>
       </c>
       <c r="K2">
-        <v>810</v>
+        <v>257</v>
       </c>
       <c r="L2">
-        <v>-18.48992474722918</v>
+        <v>-62.91272041886447</v>
       </c>
       <c r="M2">
         <v>0</v>
       </c>
       <c r="N2">
-        <v>4.355733271500807</v>
+        <v>4.355622319099083</v>
       </c>
       <c r="O2">
-        <v>5.022399938167474</v>
+        <v>5.02228898576575</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -515,46 +515,46 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>13.70805124018053</v>
+        <v>-8.0941154069587</v>
       </c>
       <c r="C3">
-        <v>73.57141012288875</v>
+        <v>9.110530214514723</v>
       </c>
       <c r="D3">
-        <v>1.136323524991484</v>
+        <v>1.378088573055627</v>
       </c>
       <c r="E3">
-        <v>-0.004722624389567093</v>
+        <v>81.22453385091053</v>
       </c>
       <c r="F3">
-        <v>-0.09075079051307866</v>
+        <v>-0.6894683831849064</v>
       </c>
       <c r="G3">
-        <v>-0.8046956967412628</v>
+        <v>-0.02385453739126353</v>
       </c>
       <c r="H3">
-        <v>0.560927550153024</v>
+        <v>0.5090568506303041</v>
       </c>
       <c r="I3">
-        <v>1.119291812005977</v>
+        <v>-0.7261686376390966</v>
       </c>
       <c r="J3">
-        <v>4.35382222130746</v>
+        <v>4.35380761793208</v>
       </c>
       <c r="K3">
-        <v>947</v>
+        <v>937</v>
       </c>
       <c r="L3">
-        <v>-18.49010939143442</v>
+        <v>-18.4904538046267</v>
       </c>
       <c r="M3">
         <v>0</v>
       </c>
       <c r="N3">
-        <v>4.355790627299218</v>
+        <v>4.355684915537104</v>
       </c>
       <c r="O3">
-        <v>5.022457293965885</v>
+        <v>5.022351582203771</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -562,46 +562,46 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>4.881855501439038e-05</v>
+        <v>30.15554940028988</v>
       </c>
       <c r="C4">
-        <v>-15.59355872078886</v>
+        <v>-159.0537175503449</v>
       </c>
       <c r="D4">
-        <v>91.89455332265962</v>
+        <v>0.1741289810405534</v>
       </c>
       <c r="E4">
-        <v>5.060803157519546</v>
+        <v>203.5577564041317</v>
       </c>
       <c r="F4">
-        <v>1.908531899953754</v>
+        <v>0.05047289782313857</v>
       </c>
       <c r="G4">
-        <v>-0.980498000492672</v>
+        <v>-0.2456751588185071</v>
       </c>
       <c r="H4">
-        <v>-0.6838360209790908</v>
+        <v>0.7346961534988825</v>
       </c>
       <c r="I4">
-        <v>0.3214507537716988</v>
+        <v>-0.3938585943787365</v>
       </c>
       <c r="J4">
-        <v>4.35373034338852</v>
+        <v>4.353778286468835</v>
       </c>
       <c r="K4">
-        <v>274</v>
+        <v>51</v>
       </c>
       <c r="L4">
-        <v>-19.77182838957472</v>
+        <v>-18.48982860918638</v>
       </c>
       <c r="M4">
         <v>0</v>
       </c>
       <c r="N4">
-        <v>4.355831438025106</v>
+        <v>4.355743674148179</v>
       </c>
       <c r="O4">
-        <v>5.022498104691773</v>
+        <v>5.022410340814846</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -609,46 +609,46 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>-18.79572377302581</v>
+        <v>10.45465227168621</v>
       </c>
       <c r="C5">
-        <v>108.0143304883464</v>
+        <v>6.169765644211846</v>
       </c>
       <c r="D5">
-        <v>82.58560653467021</v>
+        <v>4.689390985214435e-05</v>
       </c>
       <c r="E5">
-        <v>0.0206616990655788</v>
+        <v>75.44439061269631</v>
       </c>
       <c r="F5">
-        <v>-0.3944535604316779</v>
+        <v>0.2488365208279393</v>
       </c>
       <c r="G5">
-        <v>-0.5515785120814303</v>
+        <v>-0.9673196855943211</v>
       </c>
       <c r="H5">
-        <v>0.05761981773850167</v>
+        <v>1.913238163245572</v>
       </c>
       <c r="I5">
-        <v>1.035222800523765</v>
+        <v>-0.5302732929203884</v>
       </c>
       <c r="J5">
-        <v>4.353718927559044</v>
+        <v>4.353754389013545</v>
       </c>
       <c r="K5">
-        <v>666</v>
+        <v>621</v>
       </c>
       <c r="L5">
-        <v>-109.0138359232274</v>
+        <v>-33.27196597344029</v>
       </c>
       <c r="M5">
         <v>0</v>
       </c>
       <c r="N5">
-        <v>4.355874682681559</v>
+        <v>4.355746050719752</v>
       </c>
       <c r="O5">
-        <v>5.022541349348226</v>
+        <v>5.022412717386419</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -656,46 +656,46 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>71.94057355310238</v>
+        <v>26.4088679892641</v>
       </c>
       <c r="C6">
-        <v>32.22058039594563</v>
+        <v>92.41251403425821</v>
       </c>
       <c r="D6">
-        <v>0.0001373789959456304</v>
+        <v>53.52965755472344</v>
       </c>
       <c r="E6">
-        <v>146.6625828325254</v>
+        <v>0.00128606673047137</v>
       </c>
       <c r="F6">
-        <v>-1.166152362930291</v>
+        <v>-1.538403256623806</v>
       </c>
       <c r="G6">
-        <v>0.1893305969037313</v>
+        <v>-0.3838261788064343</v>
       </c>
       <c r="H6">
-        <v>1.685687279781414</v>
+        <v>0.1135073258319177</v>
       </c>
       <c r="I6">
-        <v>-0.1049567099281041</v>
+        <v>1.390909124276527</v>
       </c>
       <c r="J6">
-        <v>4.353816357952695</v>
+        <v>4.353795121719429</v>
       </c>
       <c r="K6">
-        <v>441</v>
+        <v>945</v>
       </c>
       <c r="L6">
-        <v>-161.5994162031472</v>
+        <v>-100.2990946094875</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
       <c r="N6">
-        <v>4.355906907589571</v>
+        <v>4.35574622047838</v>
       </c>
       <c r="O6">
-        <v>5.022573574256238</v>
+        <v>5.022412887145047</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -703,46 +703,46 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>15.01760889926723</v>
+        <v>0.04551887775591026</v>
       </c>
       <c r="C7">
-        <v>83.35191320937608</v>
+        <v>3.049401829752029</v>
       </c>
       <c r="D7">
-        <v>0.0006261238700516225</v>
+        <v>52.39268169665311</v>
       </c>
       <c r="E7">
-        <v>82.72617323457345</v>
+        <v>26.30273150456254</v>
       </c>
       <c r="F7">
-        <v>-0.6946099860784332</v>
+        <v>0.6794030986343471</v>
       </c>
       <c r="G7">
-        <v>-0.4954437038043416</v>
+        <v>0.3922754691060586</v>
       </c>
       <c r="H7">
-        <v>1.574032491211521</v>
+        <v>-0.7813892694683786</v>
       </c>
       <c r="I7">
-        <v>0.07315505356854901</v>
+        <v>-0.4080308380812336</v>
       </c>
       <c r="J7">
-        <v>4.353690067355402</v>
+        <v>4.353824055077897</v>
       </c>
       <c r="K7">
-        <v>186</v>
+        <v>778</v>
       </c>
       <c r="L7">
-        <v>-119.3163241619844</v>
+        <v>-18.48995982126471</v>
       </c>
       <c r="M7">
         <v>0</v>
       </c>
       <c r="N7">
-        <v>4.355930353028171</v>
+        <v>4.355755810203156</v>
       </c>
       <c r="O7">
-        <v>5.022597019694838</v>
+        <v>5.022422476869823</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -750,46 +750,46 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>63.85248572969289</v>
+        <v>2.641637624666615</v>
       </c>
       <c r="C8">
-        <v>1.445582801208831</v>
+        <v>1.266984588286954</v>
       </c>
       <c r="D8">
-        <v>19.90509115604056</v>
+        <v>17.81970626781357</v>
       </c>
       <c r="E8">
-        <v>15.64103335126555</v>
+        <v>65.82087572925903</v>
       </c>
       <c r="F8">
-        <v>-0.838818744605369</v>
+        <v>0.2133985500628559</v>
       </c>
       <c r="G8">
-        <v>0.5069442129442572</v>
+        <v>0.4984203616193201</v>
       </c>
       <c r="H8">
-        <v>-1.199429697840287</v>
+        <v>-0.3325013672918351</v>
       </c>
       <c r="I8">
-        <v>-0.1271970609481965</v>
+        <v>-0.8117430424133312</v>
       </c>
       <c r="J8">
-        <v>4.353794088132723</v>
+        <v>4.353805514627552</v>
       </c>
       <c r="K8">
-        <v>801</v>
+        <v>469</v>
       </c>
       <c r="L8">
-        <v>-18.48975571815647</v>
+        <v>-18.48968644373167</v>
       </c>
       <c r="M8">
         <v>0</v>
       </c>
       <c r="N8">
-        <v>4.355956415020117</v>
+        <v>4.355859835452137</v>
       </c>
       <c r="O8">
-        <v>5.022623081686784</v>
+        <v>5.022526502118803</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -797,46 +797,46 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>-10.67969568839464</v>
+        <v>25.91285118940834</v>
       </c>
       <c r="C9">
-        <v>0.069971217097127</v>
+        <v>0.004368737047227582</v>
       </c>
       <c r="D9">
-        <v>7.161349042059957</v>
+        <v>1.964315188081088</v>
       </c>
       <c r="E9">
-        <v>93.20732053430905</v>
+        <v>81.24557095895548</v>
       </c>
       <c r="F9">
-        <v>-0.4610328246617112</v>
+        <v>-0.08647006918719491</v>
       </c>
       <c r="G9">
-        <v>0.8571344113150654</v>
+        <v>1.041943234144266</v>
       </c>
       <c r="H9">
-        <v>0.2130926335193486</v>
+        <v>0.4566069549973326</v>
       </c>
       <c r="I9">
-        <v>-0.7067080165397148</v>
+        <v>-0.9033456813570244</v>
       </c>
       <c r="J9">
-        <v>4.353734053836256</v>
+        <v>4.353778999871952</v>
       </c>
       <c r="K9">
-        <v>219</v>
+        <v>802</v>
       </c>
       <c r="L9">
-        <v>-18.48998246241425</v>
+        <v>-28.72136330555168</v>
       </c>
       <c r="M9">
         <v>0</v>
       </c>
       <c r="N9">
-        <v>4.355977773038699</v>
+        <v>4.355939097714391</v>
       </c>
       <c r="O9">
-        <v>5.022644439705366</v>
+        <v>5.022605764381058</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -844,46 +844,46 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>12.59202612535058</v>
+        <v>0.1779081014491591</v>
       </c>
       <c r="C10">
-        <v>2.949494921891286</v>
+        <v>-93.40243263581021</v>
       </c>
       <c r="D10">
-        <v>0.2559593421907637</v>
+        <v>170.7072061467497</v>
       </c>
       <c r="E10">
-        <v>82.92236675692584</v>
+        <v>34.91794191928116</v>
       </c>
       <c r="F10">
-        <v>-0.1587343389394977</v>
+        <v>0.7557727624322843</v>
       </c>
       <c r="G10">
-        <v>0.298164239586872</v>
+        <v>-1.04992582854416</v>
       </c>
       <c r="H10">
-        <v>0.6808302357053031</v>
+        <v>-0.8621751461306277</v>
       </c>
       <c r="I10">
-        <v>-0.8756000411091078</v>
+        <v>0.06158433865995638</v>
       </c>
       <c r="J10">
-        <v>4.353766400874147</v>
+        <v>4.35371795186191</v>
       </c>
       <c r="K10">
-        <v>197</v>
+        <v>526</v>
       </c>
       <c r="L10">
-        <v>-18.50061651607908</v>
+        <v>-48.06299196929407</v>
       </c>
       <c r="M10">
         <v>0</v>
       </c>
       <c r="N10">
-        <v>4.356025606750617</v>
+        <v>4.355946107051409</v>
       </c>
       <c r="O10">
-        <v>5.022692273417284</v>
+        <v>5.022612773718076</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -891,46 +891,46 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>76.16162303422527</v>
+        <v>1.348284501574201</v>
       </c>
       <c r="C11">
-        <v>120.8958378571488</v>
+        <v>2.714814759204617e-06</v>
       </c>
       <c r="D11">
-        <v>38.71805380907443</v>
+        <v>92.84530405557746</v>
       </c>
       <c r="E11">
-        <v>0.06937189547648326</v>
+        <v>24.44006165666981</v>
       </c>
       <c r="F11">
-        <v>-0.8237584855118192</v>
+        <v>0.5223596406124948</v>
       </c>
       <c r="G11">
-        <v>0.0430167232194969</v>
+        <v>1.697505301138365</v>
       </c>
       <c r="H11">
-        <v>-0.2269302406879004</v>
+        <v>-1.114819023889696</v>
       </c>
       <c r="I11">
-        <v>0.8737592316565159</v>
+        <v>-0.2036030782800891</v>
       </c>
       <c r="J11">
-        <v>4.353730130279445</v>
+        <v>4.353815200091578</v>
       </c>
       <c r="K11">
-        <v>994</v>
+        <v>98</v>
       </c>
       <c r="L11">
-        <v>-160.0330460197437</v>
+        <v>-18.50677047089281</v>
       </c>
       <c r="M11">
         <v>0</v>
       </c>
       <c r="N11">
-        <v>4.356025841023182</v>
+        <v>4.356042197637365</v>
       </c>
       <c r="O11">
-        <v>5.022692507689849</v>
+        <v>5.022708864304032</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrections targetfolder (result printing)
trials 99% complete (absence reference targetfolder Phase5)

next: automate LN-approximation
later: auto-visualize PDF; CDF; cCDF and LN approx
</commit_message>
<xml_diff>
--- a/Tester.xlsx
+++ b/Tester.xlsx
@@ -468,46 +468,46 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.007921659358885036</v>
+        <v>-9.361830160744564</v>
       </c>
       <c r="C2">
-        <v>104.7277239638582</v>
+        <v>79.9214580198452</v>
       </c>
       <c r="D2">
-        <v>-76.12851921821058</v>
+        <v>8.109283971907509</v>
       </c>
       <c r="E2">
-        <v>86.83826899324438</v>
+        <v>5.449597197199146e-05</v>
       </c>
       <c r="F2">
-        <v>1.087736738464413</v>
+        <v>-1.336606832821891</v>
       </c>
       <c r="G2">
-        <v>0.137925699246686</v>
+        <v>-0.543091955582276</v>
       </c>
       <c r="H2">
-        <v>0.1321353430312686</v>
+        <v>0.2818183968919779</v>
       </c>
       <c r="I2">
-        <v>-0.457978408653416</v>
+        <v>1.812345802972573</v>
       </c>
       <c r="J2">
-        <v>4.353809811669684</v>
+        <v>4.353799460192466</v>
       </c>
       <c r="K2">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="L2">
-        <v>-62.91272041886447</v>
+        <v>-29.8862848846466</v>
       </c>
       <c r="M2">
         <v>0</v>
       </c>
       <c r="N2">
-        <v>4.355622319099083</v>
+        <v>4.355584533945237</v>
       </c>
       <c r="O2">
-        <v>5.02228898576575</v>
+        <v>5.022251200611904</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -515,46 +515,46 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>-8.0941154069587</v>
+        <v>6.596534342844713</v>
       </c>
       <c r="C3">
-        <v>9.110530214514723</v>
+        <v>1.825852598549732</v>
       </c>
       <c r="D3">
-        <v>1.378088573055627</v>
+        <v>0.0001378031027128604</v>
       </c>
       <c r="E3">
-        <v>81.22453385091053</v>
+        <v>75.20885893170779</v>
       </c>
       <c r="F3">
-        <v>-0.6894683831849064</v>
+        <v>0.2961473385211364</v>
       </c>
       <c r="G3">
-        <v>-0.02385453739126353</v>
+        <v>-0.6011903421046492</v>
       </c>
       <c r="H3">
-        <v>0.5090568506303041</v>
+        <v>1.707038627490326</v>
       </c>
       <c r="I3">
-        <v>-0.7261686376390966</v>
+        <v>-0.5890721322461243</v>
       </c>
       <c r="J3">
-        <v>4.35380761793208</v>
+        <v>4.353762573808641</v>
       </c>
       <c r="K3">
-        <v>937</v>
+        <v>353</v>
       </c>
       <c r="L3">
-        <v>-18.4904538046267</v>
+        <v>-24.69881904272587</v>
       </c>
       <c r="M3">
         <v>0</v>
       </c>
       <c r="N3">
-        <v>4.355684915537104</v>
+        <v>4.35572411496149</v>
       </c>
       <c r="O3">
-        <v>5.022351582203771</v>
+        <v>5.022390781628157</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -562,46 +562,46 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>30.15554940028988</v>
+        <v>0.0003578390485837374</v>
       </c>
       <c r="C4">
-        <v>-159.0537175503449</v>
+        <v>26.48330213504671</v>
       </c>
       <c r="D4">
-        <v>0.1741289810405534</v>
+        <v>74.18715757271076</v>
       </c>
       <c r="E4">
-        <v>203.5577564041317</v>
+        <v>2.768469704767545</v>
       </c>
       <c r="F4">
-        <v>0.05047289782313857</v>
+        <v>1.455781544625709</v>
       </c>
       <c r="G4">
-        <v>-0.2456751588185071</v>
+        <v>-0.009869048897695798</v>
       </c>
       <c r="H4">
-        <v>0.7346961534988825</v>
+        <v>-0.6828996761626946</v>
       </c>
       <c r="I4">
-        <v>-0.3938585943787365</v>
+        <v>0.4053679610471881</v>
       </c>
       <c r="J4">
-        <v>4.353778286468835</v>
+        <v>4.353781715690026</v>
       </c>
       <c r="K4">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="L4">
-        <v>-18.48982860918638</v>
+        <v>-40.13340457506403</v>
       </c>
       <c r="M4">
         <v>0</v>
       </c>
       <c r="N4">
-        <v>4.355743674148179</v>
+        <v>4.355733012259954</v>
       </c>
       <c r="O4">
-        <v>5.022410340814846</v>
+        <v>5.022399678926621</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -609,46 +609,46 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>10.45465227168621</v>
+        <v>7.235222724324111</v>
       </c>
       <c r="C5">
-        <v>6.169765644211846</v>
+        <v>1.823592883824094</v>
       </c>
       <c r="D5">
-        <v>4.689390985214435e-05</v>
+        <v>0.1732319419628537</v>
       </c>
       <c r="E5">
-        <v>75.44439061269631</v>
+        <v>74.46176761665646</v>
       </c>
       <c r="F5">
-        <v>0.2488365208279393</v>
+        <v>0.2317875963304656</v>
       </c>
       <c r="G5">
-        <v>-0.9673196855943211</v>
+        <v>-0.6868283319011741</v>
       </c>
       <c r="H5">
-        <v>1.913238163245572</v>
+        <v>0.6997131497254809</v>
       </c>
       <c r="I5">
-        <v>-0.5302732929203884</v>
+        <v>-0.6233165677115948</v>
       </c>
       <c r="J5">
-        <v>4.353754389013545</v>
+        <v>4.353796303221486</v>
       </c>
       <c r="K5">
-        <v>621</v>
+        <v>136</v>
       </c>
       <c r="L5">
-        <v>-33.27196597344029</v>
+        <v>-23.11438027717823</v>
       </c>
       <c r="M5">
         <v>0</v>
       </c>
       <c r="N5">
-        <v>4.355746050719752</v>
+        <v>4.3557415291715</v>
       </c>
       <c r="O5">
-        <v>5.022412717386419</v>
+        <v>5.022408195838167</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -656,46 +656,46 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>26.4088679892641</v>
+        <v>2.375872132867816</v>
       </c>
       <c r="C6">
-        <v>92.41251403425821</v>
+        <v>0.0001071321012569115</v>
       </c>
       <c r="D6">
-        <v>53.52965755472344</v>
+        <v>55.21726756618601</v>
       </c>
       <c r="E6">
-        <v>0.00128606673047137</v>
+        <v>71.76632244377979</v>
       </c>
       <c r="F6">
-        <v>-1.538403256623806</v>
+        <v>0.4479931904071734</v>
       </c>
       <c r="G6">
-        <v>-0.3838261788064343</v>
+        <v>1.257083984185609</v>
       </c>
       <c r="H6">
-        <v>0.1135073258319177</v>
+        <v>-0.03676376659192426</v>
       </c>
       <c r="I6">
-        <v>1.390909124276527</v>
+        <v>-0.7983122541075389</v>
       </c>
       <c r="J6">
-        <v>4.353795121719429</v>
+        <v>4.353808698294706</v>
       </c>
       <c r="K6">
-        <v>945</v>
+        <v>774</v>
       </c>
       <c r="L6">
-        <v>-100.2990946094875</v>
+        <v>-60.6001529040814</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
       <c r="N6">
-        <v>4.35574622047838</v>
+        <v>4.355747789085157</v>
       </c>
       <c r="O6">
-        <v>5.022412887145047</v>
+        <v>5.022414455751824</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -703,46 +703,46 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.04551887775591026</v>
+        <v>16.03804488700605</v>
       </c>
       <c r="C7">
-        <v>3.049401829752029</v>
+        <v>14.49656565995068</v>
       </c>
       <c r="D7">
-        <v>52.39268169665311</v>
+        <v>74.69710326583348</v>
       </c>
       <c r="E7">
-        <v>26.30273150456254</v>
+        <v>0.07144430964662618</v>
       </c>
       <c r="F7">
-        <v>0.6794030986343471</v>
+        <v>-1.547401700763939</v>
       </c>
       <c r="G7">
-        <v>0.3922754691060586</v>
+        <v>0.1835092744198308</v>
       </c>
       <c r="H7">
-        <v>-0.7813892694683786</v>
+        <v>-0.5382717719789614</v>
       </c>
       <c r="I7">
-        <v>-0.4080308380812336</v>
+        <v>0.8114934974099586</v>
       </c>
       <c r="J7">
-        <v>4.353824055077897</v>
+        <v>4.353806728819031</v>
       </c>
       <c r="K7">
-        <v>778</v>
+        <v>974</v>
       </c>
       <c r="L7">
-        <v>-18.48995982126471</v>
+        <v>-36.45841838058163</v>
       </c>
       <c r="M7">
         <v>0</v>
       </c>
       <c r="N7">
-        <v>4.355755810203156</v>
+        <v>4.355757354098976</v>
       </c>
       <c r="O7">
-        <v>5.022422476869823</v>
+        <v>5.022424020765643</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -750,46 +750,46 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>2.641637624666615</v>
+        <v>7.676241468781314</v>
       </c>
       <c r="C8">
-        <v>1.266984588286954</v>
+        <v>21.60751300598568</v>
       </c>
       <c r="D8">
-        <v>17.81970626781357</v>
+        <v>58.38320844267371</v>
       </c>
       <c r="E8">
-        <v>65.82087572925903</v>
+        <v>0.001275615317276173</v>
       </c>
       <c r="F8">
-        <v>0.2133985500628559</v>
+        <v>0.2714940977360194</v>
       </c>
       <c r="G8">
-        <v>0.4984203616193201</v>
+        <v>-0.7794024848719248</v>
       </c>
       <c r="H8">
-        <v>-0.3325013672918351</v>
+        <v>-0.5519685565960033</v>
       </c>
       <c r="I8">
-        <v>-0.8117430424133312</v>
+        <v>1.371028643870078</v>
       </c>
       <c r="J8">
-        <v>4.353805514627552</v>
+        <v>4.353758200196836</v>
       </c>
       <c r="K8">
-        <v>469</v>
+        <v>108</v>
       </c>
       <c r="L8">
-        <v>-18.48968644373167</v>
+        <v>-26.13370530623557</v>
       </c>
       <c r="M8">
         <v>0</v>
       </c>
       <c r="N8">
-        <v>4.355859835452137</v>
+        <v>4.355764287152763</v>
       </c>
       <c r="O8">
-        <v>5.022526502118803</v>
+        <v>5.02243095381943</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -797,46 +797,46 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>25.91285118940834</v>
+        <v>0.747428462616138</v>
       </c>
       <c r="C9">
-        <v>0.004368737047227582</v>
+        <v>74.05165941048614</v>
       </c>
       <c r="D9">
-        <v>1.964315188081088</v>
+        <v>8.054987754254459</v>
       </c>
       <c r="E9">
-        <v>81.24557095895548</v>
+        <v>1.881876605834397</v>
       </c>
       <c r="F9">
-        <v>-0.08647006918719491</v>
+        <v>0.5379062400866643</v>
       </c>
       <c r="G9">
-        <v>1.041943234144266</v>
+        <v>-0.7302051705165971</v>
       </c>
       <c r="H9">
-        <v>0.4566069549973326</v>
+        <v>-0.1036781222442318</v>
       </c>
       <c r="I9">
-        <v>-0.9033456813570244</v>
+        <v>0.3298165943394573</v>
       </c>
       <c r="J9">
-        <v>4.353778999871952</v>
+        <v>4.353799575730104</v>
       </c>
       <c r="K9">
-        <v>802</v>
+        <v>961</v>
       </c>
       <c r="L9">
-        <v>-28.72136330555168</v>
+        <v>-18.48984247227505</v>
       </c>
       <c r="M9">
         <v>0</v>
       </c>
       <c r="N9">
-        <v>4.355939097714391</v>
+        <v>4.35581188612813</v>
       </c>
       <c r="O9">
-        <v>5.022605764381058</v>
+        <v>5.022478552794797</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -844,46 +844,46 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.1779081014491591</v>
+        <v>2.69765586013661</v>
       </c>
       <c r="C10">
-        <v>-93.40243263581021</v>
+        <v>80.71012257875209</v>
       </c>
       <c r="D10">
-        <v>170.7072061467497</v>
+        <v>0.8766402467110316</v>
       </c>
       <c r="E10">
-        <v>34.91794191928116</v>
+        <v>11.89895577184867</v>
       </c>
       <c r="F10">
-        <v>0.7557727624322843</v>
+        <v>0.1841065939362734</v>
       </c>
       <c r="G10">
-        <v>-1.04992582854416</v>
+        <v>-0.8541930096725487</v>
       </c>
       <c r="H10">
-        <v>-0.8621751461306277</v>
+        <v>0.5558024644633233</v>
       </c>
       <c r="I10">
-        <v>0.06158433865995638</v>
+        <v>-0.1453879663425757</v>
       </c>
       <c r="J10">
-        <v>4.35371795186191</v>
+        <v>4.353778366623544</v>
       </c>
       <c r="K10">
-        <v>526</v>
+        <v>726</v>
       </c>
       <c r="L10">
-        <v>-48.06299196929407</v>
+        <v>-18.74199211138344</v>
       </c>
       <c r="M10">
         <v>0</v>
       </c>
       <c r="N10">
-        <v>4.355946107051409</v>
+        <v>4.355977461948342</v>
       </c>
       <c r="O10">
-        <v>5.022612773718076</v>
+        <v>5.022644128615009</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -891,46 +891,46 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>1.348284501574201</v>
+        <v>0.0306258427404588</v>
       </c>
       <c r="C11">
-        <v>2.714814759204617e-06</v>
+        <v>94.34855615777451</v>
       </c>
       <c r="D11">
-        <v>92.84530405557746</v>
+        <v>-3.561242783948757</v>
       </c>
       <c r="E11">
-        <v>24.44006165666981</v>
+        <v>16.77205723344833</v>
       </c>
       <c r="F11">
-        <v>0.5223596406124948</v>
+        <v>0.9985427644049873</v>
       </c>
       <c r="G11">
-        <v>1.697505301138365</v>
+        <v>-0.7704248316864066</v>
       </c>
       <c r="H11">
-        <v>-1.114819023889696</v>
+        <v>-1.022015410261035</v>
       </c>
       <c r="I11">
-        <v>-0.2036030782800891</v>
+        <v>0.1356312661511834</v>
       </c>
       <c r="J11">
-        <v>4.353815200091578</v>
+        <v>4.353696125234475</v>
       </c>
       <c r="K11">
-        <v>98</v>
+        <v>213</v>
       </c>
       <c r="L11">
-        <v>-18.50677047089281</v>
+        <v>-30.49242943388767</v>
       </c>
       <c r="M11">
         <v>0</v>
       </c>
       <c r="N11">
-        <v>4.356042197637365</v>
+        <v>4.356117816428284</v>
       </c>
       <c r="O11">
-        <v>5.022708864304032</v>
+        <v>5.022784483094951</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PhaseSix auto-visualization included in standard procedure
Rerun of test-cases ongoing.

To do:
- m=4 currently hardcoded, m-indication should be included in output Phase4
- calc K-L divergence (or similar) of ME-MDRM and MDRM-G => decision measure
- improve optimization algorithm
- fix LHS alpha values for repeatability
</commit_message>
<xml_diff>
--- a/Tester.xlsx
+++ b/Tester.xlsx
@@ -468,46 +468,46 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>-9.361830160744564</v>
+        <v>6.484760527490852</v>
       </c>
       <c r="C2">
-        <v>79.9214580198452</v>
+        <v>2.974931511405659</v>
       </c>
       <c r="D2">
-        <v>8.109283971907509</v>
+        <v>73.29250480412391</v>
       </c>
       <c r="E2">
-        <v>5.449597197199146e-05</v>
+        <v>0.001200297787319263</v>
       </c>
       <c r="F2">
-        <v>-1.336606832821891</v>
+        <v>0.3070136037349682</v>
       </c>
       <c r="G2">
-        <v>-0.543091955582276</v>
+        <v>-1.576088003932502</v>
       </c>
       <c r="H2">
-        <v>0.2818183968919779</v>
+        <v>-0.5252816652720125</v>
       </c>
       <c r="I2">
-        <v>1.812345802972573</v>
+        <v>1.258298382116306</v>
       </c>
       <c r="J2">
-        <v>4.353799460192466</v>
+        <v>4.353833897097513</v>
       </c>
       <c r="K2">
-        <v>249</v>
+        <v>933</v>
       </c>
       <c r="L2">
-        <v>-29.8862848846466</v>
+        <v>-27.01326210292276</v>
       </c>
       <c r="M2">
         <v>0</v>
       </c>
       <c r="N2">
-        <v>4.355584533945237</v>
+        <v>4.355597361710274</v>
       </c>
       <c r="O2">
-        <v>5.022251200611904</v>
+        <v>5.022264028376941</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -515,46 +515,46 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>6.596534342844713</v>
+        <v>215.8460488256372</v>
       </c>
       <c r="C3">
-        <v>1.825852598549732</v>
+        <v>54.41977192452163</v>
       </c>
       <c r="D3">
-        <v>0.0001378031027128604</v>
+        <v>0.06296368512311659</v>
       </c>
       <c r="E3">
-        <v>75.20885893170779</v>
+        <v>-154.2868618104845</v>
       </c>
       <c r="F3">
-        <v>0.2961473385211364</v>
+        <v>-0.329547730428837</v>
       </c>
       <c r="G3">
-        <v>-0.6011903421046492</v>
+        <v>0.07897087730742713</v>
       </c>
       <c r="H3">
-        <v>1.707038627490326</v>
+        <v>0.8249624745230482</v>
       </c>
       <c r="I3">
-        <v>-0.5890721322461243</v>
+        <v>-0.2167969128771863</v>
       </c>
       <c r="J3">
-        <v>4.353762573808641</v>
+        <v>4.353822396771477</v>
       </c>
       <c r="K3">
-        <v>353</v>
+        <v>365</v>
       </c>
       <c r="L3">
-        <v>-24.69881904272587</v>
+        <v>-65.00020152445437</v>
       </c>
       <c r="M3">
         <v>0</v>
       </c>
       <c r="N3">
-        <v>4.35572411496149</v>
+        <v>4.35562456493966</v>
       </c>
       <c r="O3">
-        <v>5.022390781628157</v>
+        <v>5.022291231606327</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -562,46 +562,46 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.0003578390485837374</v>
+        <v>0.0001375871783498155</v>
       </c>
       <c r="C4">
-        <v>26.48330213504671</v>
+        <v>111.3254406937106</v>
       </c>
       <c r="D4">
-        <v>74.18715757271076</v>
+        <v>26.02470625388843</v>
       </c>
       <c r="E4">
-        <v>2.768469704767545</v>
+        <v>97.09511874251959</v>
       </c>
       <c r="F4">
-        <v>1.455781544625709</v>
+        <v>1.749804386321745</v>
       </c>
       <c r="G4">
-        <v>-0.009869048897695798</v>
+        <v>-0.331850500117137</v>
       </c>
       <c r="H4">
-        <v>-0.6828996761626946</v>
+        <v>-1.765056258813615</v>
       </c>
       <c r="I4">
-        <v>0.4053679610471881</v>
+        <v>0.08660936900193228</v>
       </c>
       <c r="J4">
-        <v>4.353781715690026</v>
+        <v>4.35382900859284</v>
       </c>
       <c r="K4">
-        <v>18</v>
+        <v>104</v>
       </c>
       <c r="L4">
-        <v>-40.13340457506403</v>
+        <v>-162.6976376054434</v>
       </c>
       <c r="M4">
         <v>0</v>
       </c>
       <c r="N4">
-        <v>4.355733012259954</v>
+        <v>4.355700516939208</v>
       </c>
       <c r="O4">
-        <v>5.022399678926621</v>
+        <v>5.022367183605875</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -609,46 +609,46 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>7.235222724324111</v>
+        <v>62.00401219989043</v>
       </c>
       <c r="C5">
-        <v>1.823592883824094</v>
+        <v>-0.0686988724152805</v>
       </c>
       <c r="D5">
-        <v>0.1732319419628537</v>
+        <v>16.81072839481216</v>
       </c>
       <c r="E5">
-        <v>74.46176761665646</v>
+        <v>2.596492926043097</v>
       </c>
       <c r="F5">
-        <v>0.2317875963304656</v>
+        <v>-0.742261392532295</v>
       </c>
       <c r="G5">
-        <v>-0.6868283319011741</v>
+        <v>0.6403693976631497</v>
       </c>
       <c r="H5">
-        <v>0.6997131497254809</v>
+        <v>-0.2935299578201138</v>
       </c>
       <c r="I5">
-        <v>-0.6233165677115948</v>
+        <v>0.4431989330853714</v>
       </c>
       <c r="J5">
-        <v>4.353796303221486</v>
+        <v>4.353829226599043</v>
       </c>
       <c r="K5">
-        <v>136</v>
+        <v>949</v>
       </c>
       <c r="L5">
-        <v>-23.11438027717823</v>
+        <v>-18.48999883258931</v>
       </c>
       <c r="M5">
         <v>0</v>
       </c>
       <c r="N5">
-        <v>4.3557415291715</v>
+        <v>4.3557377345204</v>
       </c>
       <c r="O5">
-        <v>5.022408195838167</v>
+        <v>5.022404401187067</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -656,46 +656,46 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>2.375872132867816</v>
+        <v>0.001027507922224007</v>
       </c>
       <c r="C6">
-        <v>0.0001071321012569115</v>
+        <v>1.031840058180127</v>
       </c>
       <c r="D6">
-        <v>55.21726756618601</v>
+        <v>28.58718385622127</v>
       </c>
       <c r="E6">
-        <v>71.76632244377979</v>
+        <v>87.03344124046752</v>
       </c>
       <c r="F6">
-        <v>0.4479931904071734</v>
+        <v>1.447963830809482</v>
       </c>
       <c r="G6">
-        <v>1.257083984185609</v>
+        <v>-1.229301218265868</v>
       </c>
       <c r="H6">
-        <v>-0.03676376659192426</v>
+        <v>0.1471364779517068</v>
       </c>
       <c r="I6">
-        <v>-0.7983122541075389</v>
+        <v>-0.5120584981971066</v>
       </c>
       <c r="J6">
-        <v>4.353808698294706</v>
+        <v>4.353740071341456</v>
       </c>
       <c r="K6">
-        <v>774</v>
+        <v>524</v>
       </c>
       <c r="L6">
-        <v>-60.6001529040814</v>
+        <v>-58.77571923202518</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
       <c r="N6">
-        <v>4.355747789085157</v>
+        <v>4.355760881489715</v>
       </c>
       <c r="O6">
-        <v>5.022414455751824</v>
+        <v>5.022427548156382</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -703,46 +703,46 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>16.03804488700605</v>
+        <v>46.44902483438472</v>
       </c>
       <c r="C7">
-        <v>14.49656565995068</v>
+        <v>37.09655258550981</v>
       </c>
       <c r="D7">
-        <v>74.69710326583348</v>
+        <v>0.1384490193450018</v>
       </c>
       <c r="E7">
-        <v>0.07144430964662618</v>
+        <v>3.851220908770927</v>
       </c>
       <c r="F7">
-        <v>-1.547401700763939</v>
+        <v>-0.9018521530548023</v>
       </c>
       <c r="G7">
-        <v>0.1835092744198308</v>
+        <v>-0.4844644207146638</v>
       </c>
       <c r="H7">
-        <v>-0.5382717719789614</v>
+        <v>0.6954831642038024</v>
       </c>
       <c r="I7">
-        <v>0.8114934974099586</v>
+        <v>0.3215955571925955</v>
       </c>
       <c r="J7">
-        <v>4.353806728819031</v>
+        <v>4.353801292017199</v>
       </c>
       <c r="K7">
-        <v>974</v>
+        <v>585</v>
       </c>
       <c r="L7">
-        <v>-36.45841838058163</v>
+        <v>-18.48980883694882</v>
       </c>
       <c r="M7">
         <v>0</v>
       </c>
       <c r="N7">
-        <v>4.355757354098976</v>
+        <v>4.355842516964856</v>
       </c>
       <c r="O7">
-        <v>5.022424020765643</v>
+        <v>5.022509183631523</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -750,46 +750,46 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>7.676241468781314</v>
+        <v>74.87480888822702</v>
       </c>
       <c r="C8">
-        <v>21.60751300598568</v>
+        <v>-0.421800843465856</v>
       </c>
       <c r="D8">
-        <v>58.38320844267371</v>
+        <v>95.24470402266655</v>
       </c>
       <c r="E8">
-        <v>0.001275615317276173</v>
+        <v>0.1115279975677855</v>
       </c>
       <c r="F8">
-        <v>0.2714940977360194</v>
+        <v>0.08076027322490242</v>
       </c>
       <c r="G8">
-        <v>-0.7794024848719248</v>
+        <v>0.645623834798482</v>
       </c>
       <c r="H8">
-        <v>-0.5519685565960033</v>
+        <v>-0.5332206045361556</v>
       </c>
       <c r="I8">
-        <v>1.371028643870078</v>
+        <v>0.8946585142796977</v>
       </c>
       <c r="J8">
-        <v>4.353758200196836</v>
+        <v>4.35371576955643</v>
       </c>
       <c r="K8">
-        <v>108</v>
+        <v>721</v>
       </c>
       <c r="L8">
-        <v>-26.13370530623557</v>
+        <v>-108.837569616994</v>
       </c>
       <c r="M8">
         <v>0</v>
       </c>
       <c r="N8">
-        <v>4.355764287152763</v>
+        <v>4.355846699701061</v>
       </c>
       <c r="O8">
-        <v>5.02243095381943</v>
+        <v>5.022513366367728</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -797,46 +797,46 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.747428462616138</v>
+        <v>-25.30642917605476</v>
       </c>
       <c r="C9">
-        <v>74.05165941048614</v>
+        <v>70.56436989947386</v>
       </c>
       <c r="D9">
-        <v>8.054987754254459</v>
+        <v>3.981789824980415</v>
       </c>
       <c r="E9">
-        <v>1.881876605834397</v>
+        <v>68.18925575230816</v>
       </c>
       <c r="F9">
-        <v>0.5379062400866643</v>
+        <v>-0.188233701045408</v>
       </c>
       <c r="G9">
-        <v>-0.7302051705165971</v>
+        <v>-1.040866130936773</v>
       </c>
       <c r="H9">
-        <v>-0.1036781222442318</v>
+        <v>0.3883552408162663</v>
       </c>
       <c r="I9">
-        <v>0.3298165943394573</v>
+        <v>-0.1953932198606885</v>
       </c>
       <c r="J9">
-        <v>4.353799575730104</v>
+        <v>4.353839073164195</v>
       </c>
       <c r="K9">
-        <v>961</v>
+        <v>376</v>
       </c>
       <c r="L9">
-        <v>-18.48984247227505</v>
+        <v>-34.92325937647293</v>
       </c>
       <c r="M9">
         <v>0</v>
       </c>
       <c r="N9">
-        <v>4.35581188612813</v>
+        <v>4.355936935495713</v>
       </c>
       <c r="O9">
-        <v>5.022478552794797</v>
+        <v>5.02260360216238</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -844,46 +844,46 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>2.69765586013661</v>
+        <v>119.7326409213468</v>
       </c>
       <c r="C10">
-        <v>80.71012257875209</v>
+        <v>81.94047024097438</v>
       </c>
       <c r="D10">
-        <v>0.8766402467110316</v>
+        <v>85.03416273998866</v>
       </c>
       <c r="E10">
-        <v>11.89895577184867</v>
+        <v>0.0007087102803752547</v>
       </c>
       <c r="F10">
-        <v>0.1841065939362734</v>
+        <v>0.06907366095363976</v>
       </c>
       <c r="G10">
-        <v>-0.8541930096725487</v>
+        <v>-0.07227372586296976</v>
       </c>
       <c r="H10">
-        <v>0.5558024644633233</v>
+        <v>-0.5927917729632113</v>
       </c>
       <c r="I10">
-        <v>-0.1453879663425757</v>
+        <v>1.55055399719802</v>
       </c>
       <c r="J10">
-        <v>4.353778366623544</v>
+        <v>4.353691795239314</v>
       </c>
       <c r="K10">
-        <v>726</v>
+        <v>451</v>
       </c>
       <c r="L10">
-        <v>-18.74199211138344</v>
+        <v>-223.2023377832309</v>
       </c>
       <c r="M10">
         <v>0</v>
       </c>
       <c r="N10">
-        <v>4.355977461948342</v>
+        <v>4.355944973611741</v>
       </c>
       <c r="O10">
-        <v>5.022644128615009</v>
+        <v>5.022611640278408</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -891,46 +891,46 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.0306258427404588</v>
+        <v>0.5753863727734907</v>
       </c>
       <c r="C11">
-        <v>94.34855615777451</v>
+        <v>0.1205574064483508</v>
       </c>
       <c r="D11">
-        <v>-3.561242783948757</v>
+        <v>85.2498340834572</v>
       </c>
       <c r="E11">
-        <v>16.77205723344833</v>
+        <v>8.632410031552443</v>
       </c>
       <c r="F11">
-        <v>0.9985427644049873</v>
+        <v>0.2522334519041363</v>
       </c>
       <c r="G11">
-        <v>-0.7704248316864066</v>
+        <v>0.7961275668097332</v>
       </c>
       <c r="H11">
-        <v>-1.022015410261035</v>
+        <v>-0.7589242339494804</v>
       </c>
       <c r="I11">
-        <v>0.1356312661511834</v>
+        <v>0.1628426857156886</v>
       </c>
       <c r="J11">
-        <v>4.353696125234475</v>
+        <v>4.353735884756489</v>
       </c>
       <c r="K11">
-        <v>213</v>
+        <v>534</v>
       </c>
       <c r="L11">
-        <v>-30.49242943388767</v>
+        <v>-20.85345408414249</v>
       </c>
       <c r="M11">
         <v>0</v>
       </c>
       <c r="N11">
-        <v>4.356117816428284</v>
+        <v>4.355987731520631</v>
       </c>
       <c r="O11">
-        <v>5.022784483094951</v>
+        <v>5.022654398187298</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add Parameter printing to Phase4, for ease of reference mean,std,cov
</commit_message>
<xml_diff>
--- a/Tester.xlsx
+++ b/Tester.xlsx
@@ -468,46 +468,46 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>12.89953091859238</v>
+        <v>0.002833900968242052</v>
       </c>
       <c r="C2">
-        <v>0.0007872700435241044</v>
+        <v>-5864.14666073515</v>
       </c>
       <c r="D2">
-        <v>42.42763100046575</v>
+        <v>-115.1647534024966</v>
       </c>
       <c r="E2">
-        <v>39.92110297930766</v>
+        <v>51410.93713904079</v>
       </c>
       <c r="F2">
-        <v>0.2269241961236386</v>
+        <v>1.596731641488282</v>
       </c>
       <c r="G2">
-        <v>1.433159681014691</v>
+        <v>-1.233552899527711</v>
       </c>
       <c r="H2">
-        <v>-0.4266104988450869</v>
+        <v>0.06949803370384533</v>
       </c>
       <c r="I2">
-        <v>-0.6328505463641105</v>
+        <v>-1.68783007370961</v>
       </c>
       <c r="J2">
-        <v>4.353781016801733</v>
+        <v>4.708258456577482</v>
       </c>
       <c r="K2">
-        <v>499</v>
+        <v>288</v>
       </c>
       <c r="L2">
-        <v>-38.80643958845396</v>
+        <v>160.13036782199</v>
       </c>
       <c r="M2">
         <v>0</v>
       </c>
       <c r="N2">
-        <v>4.355671628393388</v>
+        <v>4.708258456577482</v>
       </c>
       <c r="O2">
-        <v>5.022338295060055</v>
+        <v>5.374925123244149</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -515,46 +515,46 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>78.29214762893965</v>
+        <v>-346.4544766790139</v>
       </c>
       <c r="C3">
-        <v>0.03097609872673852</v>
+        <v>-5138.16875532128</v>
       </c>
       <c r="D3">
-        <v>10.16513911934931</v>
+        <v>13318.72736983711</v>
       </c>
       <c r="E3">
-        <v>-1.566980884799998</v>
+        <v>0.0001857736446508796</v>
       </c>
       <c r="F3">
-        <v>-0.5847605532197486</v>
+        <v>-0.6405017168990723</v>
       </c>
       <c r="G3">
-        <v>0.9092197743984984</v>
+        <v>-1.551981812672806</v>
       </c>
       <c r="H3">
-        <v>0.2255827633484868</v>
+        <v>-1.341692803832187</v>
       </c>
       <c r="I3">
-        <v>-1.603148225604978</v>
+        <v>1.989389935750627</v>
       </c>
       <c r="J3">
-        <v>4.353787634385213</v>
+        <v>4.708273077746254</v>
       </c>
       <c r="K3">
-        <v>392</v>
+        <v>581</v>
       </c>
       <c r="L3">
-        <v>-29.49644937834564</v>
+        <v>0.39099350149622</v>
       </c>
       <c r="M3">
         <v>0</v>
       </c>
       <c r="N3">
-        <v>4.355710135658569</v>
+        <v>4.708273077746261</v>
       </c>
       <c r="O3">
-        <v>5.022376802325236</v>
+        <v>5.374939744412928</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -562,46 +562,46 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>26.73965786837452</v>
+        <v>-12937.70730302205</v>
       </c>
       <c r="C4">
-        <v>0.0005012382834615374</v>
+        <v>0.0009968436357354659</v>
       </c>
       <c r="D4">
-        <v>38.54168610435296</v>
+        <v>13315.72371925506</v>
       </c>
       <c r="E4">
-        <v>88.03715010904722</v>
+        <v>22073.55800362063</v>
       </c>
       <c r="F4">
-        <v>-1.353590237368841</v>
+        <v>-1.017822263739436</v>
       </c>
       <c r="G4">
-        <v>1.522507241321895</v>
+        <v>1.729893523390114</v>
       </c>
       <c r="H4">
-        <v>0.1416705823448821</v>
+        <v>-1.013779453922141</v>
       </c>
       <c r="I4">
-        <v>-0.3619050437573446</v>
+        <v>-1.695854597040008</v>
       </c>
       <c r="J4">
-        <v>4.353797881712794</v>
+        <v>4.708281036686117</v>
       </c>
       <c r="K4">
-        <v>739</v>
+        <v>52</v>
       </c>
       <c r="L4">
-        <v>-84.67974108613107</v>
+        <v>-10.03184155721563</v>
       </c>
       <c r="M4">
         <v>0</v>
       </c>
       <c r="N4">
-        <v>4.355726530908555</v>
+        <v>4.708281036718855</v>
       </c>
       <c r="O4">
-        <v>5.022393197575222</v>
+        <v>5.374947703385522</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -609,46 +609,46 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.01154578614090958</v>
+        <v>0.0007700566648021041</v>
       </c>
       <c r="C5">
-        <v>696.6217598578085</v>
+        <v>-1527.798229141081</v>
       </c>
       <c r="D5">
-        <v>-313.1327693085302</v>
+        <v>-1605.011723441246</v>
       </c>
       <c r="E5">
-        <v>103.8833258730647</v>
+        <v>9174.3002126514</v>
       </c>
       <c r="F5">
-        <v>1.101754069752864</v>
+        <v>1.7644558855894</v>
       </c>
       <c r="G5">
-        <v>0.02814569632648611</v>
+        <v>-0.8571358208756725</v>
       </c>
       <c r="H5">
-        <v>0.03622873679112759</v>
+        <v>-1.144144103285236</v>
       </c>
       <c r="I5">
-        <v>-0.4619197111338029</v>
+        <v>-1.140364276522475</v>
       </c>
       <c r="J5">
-        <v>4.353744387071742</v>
+        <v>4.708292990727894</v>
       </c>
       <c r="K5">
-        <v>228</v>
+        <v>668</v>
       </c>
       <c r="L5">
-        <v>-430.7024630528983</v>
+        <v>-5.327749651820979</v>
       </c>
       <c r="M5">
         <v>0</v>
       </c>
       <c r="N5">
-        <v>4.355756070124528</v>
+        <v>4.70829299072791</v>
       </c>
       <c r="O5">
-        <v>5.022422736791195</v>
+        <v>5.374959657394577</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -656,46 +656,46 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>69.19936063565771</v>
+        <v>0.001852846804108962</v>
       </c>
       <c r="C6">
-        <v>0.005486985206206599</v>
+        <v>-0.4202368598012528</v>
       </c>
       <c r="D6">
-        <v>5.866901637011428</v>
+        <v>-2522.329220115455</v>
       </c>
       <c r="E6">
-        <v>25.73213414892067</v>
+        <v>12197.20793857272</v>
       </c>
       <c r="F6">
-        <v>-0.5631967539309228</v>
+        <v>1.635660178183984</v>
       </c>
       <c r="G6">
-        <v>1.120371230121493</v>
+        <v>0.3736159243433201</v>
       </c>
       <c r="H6">
-        <v>0.3018764103076479</v>
+        <v>-1.720160387742061</v>
       </c>
       <c r="I6">
-        <v>-1.616595451987454</v>
+        <v>-1.455457572209112</v>
       </c>
       <c r="J6">
-        <v>4.353808078793907</v>
+        <v>4.708295376414575</v>
       </c>
       <c r="K6">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="L6">
-        <v>-23.13665350323468</v>
+        <v>-7.59671641329339</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
       <c r="N6">
-        <v>4.355783027185492</v>
+        <v>4.708295376432961</v>
       </c>
       <c r="O6">
-        <v>5.022449693852159</v>
+        <v>5.374962043099628</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -703,46 +703,46 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.003051293888421791</v>
+        <v>-3497.990009461215</v>
       </c>
       <c r="C7">
-        <v>-14.91608721405803</v>
+        <v>0.0006923256595945056</v>
       </c>
       <c r="D7">
-        <v>34.49105225234221</v>
+        <v>-3996.847146262389</v>
       </c>
       <c r="E7">
-        <v>96.46044324275883</v>
+        <v>31202.40295610447</v>
       </c>
       <c r="F7">
-        <v>1.298823116519899</v>
+        <v>-1.460960037463827</v>
       </c>
       <c r="G7">
-        <v>-0.1760232982482453</v>
+        <v>1.780521669734684</v>
       </c>
       <c r="H7">
-        <v>0.1198301572060605</v>
+        <v>-1.750540777755884</v>
       </c>
       <c r="I7">
-        <v>-0.5112038820556393</v>
+        <v>-1.621809611138783</v>
       </c>
       <c r="J7">
-        <v>4.353725449452583</v>
+        <v>4.708307027130176</v>
       </c>
       <c r="K7">
-        <v>927</v>
+        <v>243</v>
       </c>
       <c r="L7">
-        <v>-57.06900089391348</v>
+        <v>-7.246890860550308</v>
       </c>
       <c r="M7">
         <v>0</v>
       </c>
       <c r="N7">
-        <v>4.355804622571981</v>
+        <v>4.708307027176368</v>
       </c>
       <c r="O7">
-        <v>5.022471289238648</v>
+        <v>5.374973693843035</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -750,46 +750,46 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>1.119196941165729</v>
+        <v>0.0005149403881635328</v>
       </c>
       <c r="C8">
-        <v>4.607699116368453</v>
+        <v>-1103.912773063059</v>
       </c>
       <c r="D8">
-        <v>49.51387989200745</v>
+        <v>-177.7457372487873</v>
       </c>
       <c r="E8">
-        <v>28.38280349514767</v>
+        <v>3514.499383008041</v>
       </c>
       <c r="F8">
-        <v>0.5120123496014859</v>
+        <v>1.810488400907328</v>
       </c>
       <c r="G8">
-        <v>0.158242362797234</v>
+        <v>-1.389026765483945</v>
       </c>
       <c r="H8">
-        <v>-0.7624202827494515</v>
+        <v>-0.1917547081398894</v>
       </c>
       <c r="I8">
-        <v>-0.5553273991564449</v>
+        <v>-0.9945498152204615</v>
       </c>
       <c r="J8">
-        <v>4.353804061071251</v>
+        <v>4.708315618662134</v>
       </c>
       <c r="K8">
-        <v>460</v>
+        <v>730</v>
       </c>
       <c r="L8">
-        <v>-18.48966510965653</v>
+        <v>44.71980227531387</v>
       </c>
       <c r="M8">
         <v>0</v>
       </c>
       <c r="N8">
-        <v>4.355837099547575</v>
+        <v>4.708315618662155</v>
       </c>
       <c r="O8">
-        <v>5.022503766214242</v>
+        <v>5.374982285328822</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -797,46 +797,46 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.0004746840785504123</v>
+        <v>0.0006533019421955117</v>
       </c>
       <c r="C9">
-        <v>49.26672235207124</v>
+        <v>515.8497165115939</v>
       </c>
       <c r="D9">
-        <v>83.28222986079379</v>
+        <v>2500.740130313069</v>
       </c>
       <c r="E9">
-        <v>77.20035803806186</v>
+        <v>70.71432700333804</v>
       </c>
       <c r="F9">
-        <v>1.592248305033589</v>
+        <v>1.768126010259178</v>
       </c>
       <c r="G9">
-        <v>-0.9612352356117611</v>
+        <v>-1.34773997977639</v>
       </c>
       <c r="H9">
-        <v>-0.2697397859904047</v>
+        <v>-0.9792683194705409</v>
       </c>
       <c r="I9">
-        <v>0.09362209295631807</v>
+        <v>0.08659808241459199</v>
       </c>
       <c r="J9">
-        <v>4.353727542890283</v>
+        <v>4.708322286540437</v>
       </c>
       <c r="K9">
-        <v>766</v>
+        <v>868</v>
       </c>
       <c r="L9">
-        <v>-137.619557013205</v>
+        <v>-128.5995452926111</v>
       </c>
       <c r="M9">
         <v>0</v>
       </c>
       <c r="N9">
-        <v>4.355955053385571</v>
+        <v>4.708322738314763</v>
       </c>
       <c r="O9">
-        <v>5.022621720052238</v>
+        <v>5.37498940498143</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -844,46 +844,46 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>-197.427803536788</v>
+        <v>-119.2465728251387</v>
       </c>
       <c r="C10">
-        <v>377.2149911829689</v>
+        <v>-507.4873829367511</v>
       </c>
       <c r="D10">
-        <v>166.868115171693</v>
+        <v>0.0001347548805125384</v>
       </c>
       <c r="E10">
-        <v>0.6809997077783453</v>
+        <v>1770.022216781039</v>
       </c>
       <c r="F10">
-        <v>-0.2208295061213041</v>
+        <v>-1.502315923047965</v>
       </c>
       <c r="G10">
-        <v>-0.02792398422629838</v>
+        <v>-0.07101887494854675</v>
       </c>
       <c r="H10">
-        <v>-0.5150578548357763</v>
+        <v>1.997798873210352</v>
       </c>
       <c r="I10">
-        <v>0.6060288088375021</v>
+        <v>-0.735354022113498</v>
       </c>
       <c r="J10">
-        <v>4.35373515433389</v>
+        <v>4.708327547191402</v>
       </c>
       <c r="K10">
-        <v>199</v>
+        <v>606</v>
       </c>
       <c r="L10">
-        <v>-280.3928191438023</v>
+        <v>312.3899551840778</v>
       </c>
       <c r="M10">
         <v>0</v>
       </c>
       <c r="N10">
-        <v>4.355973341649417</v>
+        <v>4.708327547191459</v>
       </c>
       <c r="O10">
-        <v>5.022640008316084</v>
+        <v>5.374994213858126</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -891,46 +891,46 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>-9.681193256260897</v>
+        <v>-277.5314346699907</v>
       </c>
       <c r="C11">
-        <v>92.78987887378455</v>
+        <v>0.003968030574984961</v>
       </c>
       <c r="D11">
-        <v>0.0004161381780290052</v>
+        <v>-6.570812047035906</v>
       </c>
       <c r="E11">
-        <v>9.982540049878637</v>
+        <v>2873.465122083891</v>
       </c>
       <c r="F11">
-        <v>-1.023363823716117</v>
+        <v>-0.3157809265194105</v>
       </c>
       <c r="G11">
-        <v>-0.6838677697679796</v>
+        <v>1.515354533756579</v>
       </c>
       <c r="H11">
-        <v>1.619640542824919</v>
+        <v>0.2601848759091361</v>
       </c>
       <c r="I11">
-        <v>0.2310771144409509</v>
+        <v>-0.9331410691209625</v>
       </c>
       <c r="J11">
-        <v>4.353692218844277</v>
+        <v>4.708329508185642</v>
       </c>
       <c r="K11">
-        <v>831</v>
+        <v>477</v>
       </c>
       <c r="L11">
-        <v>-26.99318292225294</v>
+        <v>50.81299256860409</v>
       </c>
       <c r="M11">
         <v>0</v>
       </c>
       <c r="N11">
-        <v>4.355983021068486</v>
+        <v>4.708329508185649</v>
       </c>
       <c r="O11">
-        <v>5.022649687735153</v>
+        <v>5.374996174852316</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated MaxEnt_sampling.py file for 'developer use'
=> option to add mean value evaluation at end of SamplingScheme
(ModelInput sheet MDRMGauss_samples.xlsx)
</commit_message>
<xml_diff>
--- a/Tester.xlsx
+++ b/Tester.xlsx
@@ -468,46 +468,46 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.002833900968242052</v>
+        <v>20.86404034540688</v>
       </c>
       <c r="C2">
-        <v>-5864.14666073515</v>
+        <v>-0.2648023883583657</v>
       </c>
       <c r="D2">
-        <v>-115.1647534024966</v>
+        <v>-59.63165798589831</v>
       </c>
       <c r="E2">
-        <v>51410.93713904079</v>
+        <v>11.58017979786816</v>
       </c>
       <c r="F2">
-        <v>1.596731641488282</v>
+        <v>-0.01942229598401335</v>
       </c>
       <c r="G2">
-        <v>-1.233552899527711</v>
+        <v>1.294366342780368</v>
       </c>
       <c r="H2">
-        <v>0.06949803370384533</v>
+        <v>0.5265508224156252</v>
       </c>
       <c r="I2">
-        <v>-1.68783007370961</v>
+        <v>0.8449859115444958</v>
       </c>
       <c r="J2">
-        <v>4.708258456577482</v>
+        <v>4.294876943500668</v>
       </c>
       <c r="K2">
-        <v>288</v>
+        <v>90</v>
       </c>
       <c r="L2">
-        <v>160.13036782199</v>
+        <v>195.0057849092381</v>
       </c>
       <c r="M2">
         <v>0</v>
       </c>
       <c r="N2">
-        <v>4.708258456577482</v>
+        <v>4.294876943485406</v>
       </c>
       <c r="O2">
-        <v>5.374925123244149</v>
+        <v>4.961543610152073</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -515,46 +515,46 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>-346.4544766790139</v>
+        <v>8.437706782665778</v>
       </c>
       <c r="C3">
-        <v>-5138.16875532128</v>
+        <v>-62.07474757071336</v>
       </c>
       <c r="D3">
-        <v>13318.72736983711</v>
+        <v>40.6684537137988</v>
       </c>
       <c r="E3">
-        <v>0.0001857736446508796</v>
+        <v>-6.149093826052811</v>
       </c>
       <c r="F3">
-        <v>-0.6405017168990723</v>
+        <v>1.134191514785718</v>
       </c>
       <c r="G3">
-        <v>-1.551981812672806</v>
+        <v>0.4046636615046872</v>
       </c>
       <c r="H3">
-        <v>-1.341692803832187</v>
+        <v>-0.2922933614285586</v>
       </c>
       <c r="I3">
-        <v>1.989389935750627</v>
+        <v>1.175201255881039</v>
       </c>
       <c r="J3">
-        <v>4.708273077746254</v>
+        <v>4.294881385958519</v>
       </c>
       <c r="K3">
-        <v>581</v>
+        <v>745</v>
       </c>
       <c r="L3">
-        <v>0.39099350149622</v>
+        <v>206.7617367230539</v>
       </c>
       <c r="M3">
         <v>0</v>
       </c>
       <c r="N3">
-        <v>4.708273077746261</v>
+        <v>4.294881385941409</v>
       </c>
       <c r="O3">
-        <v>5.374939744412928</v>
+        <v>4.961548052608076</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -562,46 +562,46 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>-12937.70730302205</v>
+        <v>1.922361242592085</v>
       </c>
       <c r="C4">
-        <v>0.0009968436357354659</v>
+        <v>-97.76669692973437</v>
       </c>
       <c r="D4">
-        <v>13315.72371925506</v>
+        <v>-0.5066926708507814</v>
       </c>
       <c r="E4">
-        <v>22073.55800362063</v>
+        <v>254.3320468013589</v>
       </c>
       <c r="F4">
-        <v>-1.017822263739436</v>
+        <v>1.136628546200298</v>
       </c>
       <c r="G4">
-        <v>1.729893523390114</v>
+        <v>0.3306943302220215</v>
       </c>
       <c r="H4">
-        <v>-1.013779453922141</v>
+        <v>1.314308009811612</v>
       </c>
       <c r="I4">
-        <v>-1.695854597040008</v>
+        <v>0.04103570621144703</v>
       </c>
       <c r="J4">
-        <v>4.708281036686117</v>
+        <v>4.294882778572594</v>
       </c>
       <c r="K4">
-        <v>52</v>
+        <v>178</v>
       </c>
       <c r="L4">
-        <v>-10.03184155721563</v>
+        <v>0.5063523926838996</v>
       </c>
       <c r="M4">
         <v>0</v>
       </c>
       <c r="N4">
-        <v>4.708281036718855</v>
+        <v>4.294882778506425</v>
       </c>
       <c r="O4">
-        <v>5.374947703385522</v>
+        <v>4.961549445173092</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -609,46 +609,46 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.0007700566648021041</v>
+        <v>8.07113803938401</v>
       </c>
       <c r="C5">
-        <v>-1527.798229141081</v>
+        <v>13.78439248856992</v>
       </c>
       <c r="D5">
-        <v>-1605.011723441246</v>
+        <v>-57.79034922294563</v>
       </c>
       <c r="E5">
-        <v>9174.3002126514</v>
+        <v>-4.535673859390252</v>
       </c>
       <c r="F5">
-        <v>1.7644558855894</v>
+        <v>-0.7840237441637992</v>
       </c>
       <c r="G5">
-        <v>-0.8571358208756725</v>
+        <v>0.9565309883628963</v>
       </c>
       <c r="H5">
-        <v>-1.144144103285236</v>
+        <v>0.5305273192901323</v>
       </c>
       <c r="I5">
-        <v>-1.140364276522475</v>
+        <v>1.086810757678709</v>
       </c>
       <c r="J5">
-        <v>4.708292990727894</v>
+        <v>4.294883894736927</v>
       </c>
       <c r="K5">
-        <v>668</v>
+        <v>636</v>
       </c>
       <c r="L5">
-        <v>-5.327749651820979</v>
+        <v>217.671028137702</v>
       </c>
       <c r="M5">
         <v>0</v>
       </c>
       <c r="N5">
-        <v>4.70829299072791</v>
+        <v>4.294883894735449</v>
       </c>
       <c r="O5">
-        <v>5.374959657394577</v>
+        <v>4.961550561402116</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -656,46 +656,46 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.001852846804108962</v>
+        <v>-0.01298580615746838</v>
       </c>
       <c r="C6">
-        <v>-0.4202368598012528</v>
+        <v>37.64356387687542</v>
       </c>
       <c r="D6">
-        <v>-2522.329220115455</v>
+        <v>10.21848532590165</v>
       </c>
       <c r="E6">
-        <v>12197.20793857272</v>
+        <v>-79.24174309366001</v>
       </c>
       <c r="F6">
-        <v>1.635660178183984</v>
+        <v>1.613154733293415</v>
       </c>
       <c r="G6">
-        <v>0.3736159243433201</v>
+        <v>-1.569106211818467</v>
       </c>
       <c r="H6">
-        <v>-1.720160387742061</v>
+        <v>0.7671495865871538</v>
       </c>
       <c r="I6">
-        <v>-1.455457572209112</v>
+        <v>0.427060484680359</v>
       </c>
       <c r="J6">
-        <v>4.708295376414575</v>
+        <v>4.294884633529477</v>
       </c>
       <c r="K6">
-        <v>107</v>
+        <v>7</v>
       </c>
       <c r="L6">
-        <v>-7.59671641329339</v>
+        <v>243.1119871685546</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
       <c r="N6">
-        <v>4.708295376432961</v>
+        <v>4.294884633488721</v>
       </c>
       <c r="O6">
-        <v>5.374962043099628</v>
+        <v>4.961551300155388</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -703,46 +703,46 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>-3497.990009461215</v>
+        <v>-85.43611080278265</v>
       </c>
       <c r="C7">
-        <v>0.0006923256595945056</v>
+        <v>55.90469749137338</v>
       </c>
       <c r="D7">
-        <v>-3996.847146262389</v>
+        <v>-15.36524131791335</v>
       </c>
       <c r="E7">
-        <v>31202.40295610447</v>
+        <v>16.38683667305714</v>
       </c>
       <c r="F7">
-        <v>-1.460960037463827</v>
+        <v>0.3188722709595937</v>
       </c>
       <c r="G7">
-        <v>1.780521669734684</v>
+        <v>-1.094963603884193</v>
       </c>
       <c r="H7">
-        <v>-1.750540777755884</v>
+        <v>1.254677277674206</v>
       </c>
       <c r="I7">
-        <v>-1.621809611138783</v>
+        <v>1.246000584393504</v>
       </c>
       <c r="J7">
-        <v>4.708307027130176</v>
+        <v>4.294885279887666</v>
       </c>
       <c r="K7">
-        <v>243</v>
+        <v>663</v>
       </c>
       <c r="L7">
-        <v>-7.246890860550308</v>
+        <v>252.5837458434072</v>
       </c>
       <c r="M7">
         <v>0</v>
       </c>
       <c r="N7">
-        <v>4.708307027176368</v>
+        <v>4.294885279834574</v>
       </c>
       <c r="O7">
-        <v>5.374973693843035</v>
+        <v>4.961551946501241</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -750,46 +750,46 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.0005149403881635328</v>
+        <v>6.131427619858171</v>
       </c>
       <c r="C8">
-        <v>-1103.912773063059</v>
+        <v>-61.14243058230221</v>
       </c>
       <c r="D8">
-        <v>-177.7457372487873</v>
+        <v>-1.053497092411878</v>
       </c>
       <c r="E8">
-        <v>3514.499383008041</v>
+        <v>44.3439595214811</v>
       </c>
       <c r="F8">
-        <v>1.810488400907328</v>
+        <v>0.9748243611752598</v>
       </c>
       <c r="G8">
-        <v>-1.389026765483945</v>
+        <v>0.4601620881912822</v>
       </c>
       <c r="H8">
-        <v>-0.1917547081398894</v>
+        <v>1.193351982051471</v>
       </c>
       <c r="I8">
-        <v>-0.9945498152204615</v>
+        <v>-0.8492619740862253</v>
       </c>
       <c r="J8">
-        <v>4.708315618662134</v>
+        <v>4.294885929044256</v>
       </c>
       <c r="K8">
-        <v>730</v>
+        <v>665</v>
       </c>
       <c r="L8">
-        <v>44.71980227531387</v>
+        <v>223.3039169410303</v>
       </c>
       <c r="M8">
         <v>0</v>
       </c>
       <c r="N8">
-        <v>4.708315618662155</v>
+        <v>4.294885929040447</v>
       </c>
       <c r="O8">
-        <v>5.374982285328822</v>
+        <v>4.961552595707114</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -797,46 +797,46 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.0006533019421955117</v>
+        <v>-0.2316807757059126</v>
       </c>
       <c r="C9">
-        <v>515.8497165115939</v>
+        <v>-141.5169330320274</v>
       </c>
       <c r="D9">
-        <v>2500.740130313069</v>
+        <v>18.69937184857107</v>
       </c>
       <c r="E9">
-        <v>70.71432700333804</v>
+        <v>79.46833380072869</v>
       </c>
       <c r="F9">
-        <v>1.768126010259178</v>
+        <v>1.280859230939957</v>
       </c>
       <c r="G9">
-        <v>-1.34773997977639</v>
+        <v>0.5808229011757886</v>
       </c>
       <c r="H9">
-        <v>-0.9792683194705409</v>
+        <v>0.2666188985282694</v>
       </c>
       <c r="I9">
-        <v>0.08659808241459199</v>
+        <v>0.6848334629426271</v>
       </c>
       <c r="J9">
-        <v>4.708322286540437</v>
+        <v>4.294887713045171</v>
       </c>
       <c r="K9">
-        <v>868</v>
+        <v>960</v>
       </c>
       <c r="L9">
-        <v>-128.5995452926111</v>
+        <v>217.0586925705963</v>
       </c>
       <c r="M9">
         <v>0</v>
       </c>
       <c r="N9">
-        <v>4.708322738314763</v>
+        <v>4.29488771304446</v>
       </c>
       <c r="O9">
-        <v>5.37498940498143</v>
+        <v>4.961554379711127</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -844,46 +844,46 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>-119.2465728251387</v>
+        <v>8.714791537705295</v>
       </c>
       <c r="C10">
-        <v>-507.4873829367511</v>
+        <v>6.639560869724908</v>
       </c>
       <c r="D10">
-        <v>0.0001347548805125384</v>
+        <v>-48.0585544049658</v>
       </c>
       <c r="E10">
-        <v>1770.022216781039</v>
+        <v>-0.04123384955852044</v>
       </c>
       <c r="F10">
-        <v>-1.502315923047965</v>
+        <v>-0.7661800556879639</v>
       </c>
       <c r="G10">
-        <v>-0.07101887494854675</v>
+        <v>0.8687202762172239</v>
       </c>
       <c r="H10">
-        <v>1.997798873210352</v>
+        <v>0.5121175310915982</v>
       </c>
       <c r="I10">
-        <v>-0.735354022113498</v>
+        <v>1.505137966294176</v>
       </c>
       <c r="J10">
-        <v>4.708327547191402</v>
+        <v>4.294890227982648</v>
       </c>
       <c r="K10">
-        <v>606</v>
+        <v>333</v>
       </c>
       <c r="L10">
-        <v>312.3899551840778</v>
+        <v>192.0349742592954</v>
       </c>
       <c r="M10">
         <v>0</v>
       </c>
       <c r="N10">
-        <v>4.708327547191459</v>
+        <v>4.29489022789582</v>
       </c>
       <c r="O10">
-        <v>5.374994213858126</v>
+        <v>4.961556894562487</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -891,46 +891,46 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>-277.5314346699907</v>
+        <v>37.60218506007669</v>
       </c>
       <c r="C11">
-        <v>0.003968030574984961</v>
+        <v>43.6097037135478</v>
       </c>
       <c r="D11">
-        <v>-6.570812047035906</v>
+        <v>-0.01234836859628072</v>
       </c>
       <c r="E11">
-        <v>2873.465122083891</v>
+        <v>-116.1705281896398</v>
       </c>
       <c r="F11">
-        <v>-0.3157809265194105</v>
+        <v>0.6442768432798145</v>
       </c>
       <c r="G11">
-        <v>1.515354533756579</v>
+        <v>-1.635924215906726</v>
       </c>
       <c r="H11">
-        <v>0.2601848759091361</v>
+        <v>1.60114082179294</v>
       </c>
       <c r="I11">
-        <v>-0.9331410691209625</v>
+        <v>0.4612304063149804</v>
       </c>
       <c r="J11">
-        <v>4.708329508185642</v>
+        <v>4.294890926946607</v>
       </c>
       <c r="K11">
-        <v>477</v>
+        <v>777</v>
       </c>
       <c r="L11">
-        <v>50.81299256860409</v>
+        <v>265.2849318004681</v>
       </c>
       <c r="M11">
         <v>0</v>
       </c>
       <c r="N11">
-        <v>4.708329508185649</v>
+        <v>4.294890926938422</v>
       </c>
       <c r="O11">
-        <v>5.374996174852316</v>
+        <v>4.961557593605089</v>
       </c>
     </row>
   </sheetData>

</xml_diff>